<commit_message>
added ghia comparison picture and solution contours for README.md
</commit_message>
<xml_diff>
--- a/data/Ghia_comparison.xlsx
+++ b/data/Ghia_comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilo\Google Drive\School\UT\Fall2019\Fall 2019\MIE1210_CFD\Project\Lid_Driven_Cavity\source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilo\Google Drive\Projects\CFD\Lid_Driven_Cavity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>P</t>
   </si>
@@ -80,10 +80,10 @@
     <t>ZONE</t>
   </si>
   <si>
-    <t>Ghia 129 x 129</t>
+    <t>70x70</t>
   </si>
   <si>
-    <t>70x70</t>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -235,7 +235,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ghia 129 x 129</c:v>
+                  <c:v>Ghia 129x129</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -585,7 +585,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0524-491F-A39D-4E3A5424AEB8}"/>
             </c:ext>
@@ -1065,12 +1065,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="525237320"/>
-        <c:axId val="525233792"/>
+        <c:axId val="216051352"/>
+        <c:axId val="421972920"/>
         <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="525237320"/>
+        <c:axId val="216051352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1158,12 +1158,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="525233792"/>
+        <c:crossAx val="421972920"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="525233792"/>
+        <c:axId val="421972920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1257,7 +1257,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="525237320"/>
+        <c:crossAx val="216051352"/>
         <c:crossesAt val="-0.5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1318,12 +1318,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1935,7 +1930,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0524-491F-A39D-4E3A5424AEB8}"/>
             </c:ext>
@@ -2117,12 +2112,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="421392808"/>
-        <c:axId val="421393984"/>
+        <c:axId val="392430664"/>
+        <c:axId val="392431056"/>
         <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="421392808"/>
+        <c:axId val="392430664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2210,12 +2205,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421393984"/>
+        <c:crossAx val="392431056"/>
         <c:crossesAt val="-0.30000000000000004"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="421393984"/>
+        <c:axId val="392431056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2302,7 +2297,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421392808"/>
+        <c:crossAx val="392430664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2364,12 +2359,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -3657,15 +3647,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>224973</xdr:colOff>
+      <xdr:colOff>220088</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>4884</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>277773</xdr:colOff>
+      <xdr:colOff>272888</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>109450</xdr:rowOff>
+      <xdr:rowOff>114334</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3990,8 +3980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A34:AM297"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="E37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4041,7 +4031,7 @@
         <v>0.17468354430379701</v>
       </c>
       <c r="AB39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AF39" t="s">
         <v>7</v>
@@ -4057,6 +4047,9 @@
       <c r="B40">
         <v>0.170886075949367</v>
       </c>
+      <c r="T40" t="s">
+        <v>19</v>
+      </c>
       <c r="AB40" t="s">
         <v>4</v>
       </c>
@@ -4929,10 +4922,10 @@
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.35">
       <c r="G60" t="s">
+        <v>8</v>
+      </c>
+      <c r="J60" t="s">
         <v>18</v>
-      </c>
-      <c r="J60" t="s">
-        <v>19</v>
       </c>
       <c r="O60" t="s">
         <v>17</v>

</xml_diff>